<commit_message>
updating ctf stuff ...
</commit_message>
<xml_diff>
--- a/sundries/ctf/2023/picoCTF/scoreboard.xlsx
+++ b/sundries/ctf/2023/picoCTF/scoreboard.xlsx
@@ -8,18 +8,182 @@
     <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="0" val="1062" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="0" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="0"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="0"/>
+      <pm:revision xmlns:pm="smNativeData" day="1680047966" val="1062" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1680047966" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1680047966" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1680047966"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+  <si>
+    <t>Rank #</t>
+  </si>
+  <si>
+    <t>Player/Team Name</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>redpwn</t>
+  </si>
+  <si>
+    <t>pb1c_jar</t>
+  </si>
+  <si>
+    <t>crusaders of redpwn jr</t>
+  </si>
+  <si>
+    <t>voltara</t>
+  </si>
+  <si>
+    <t>YegSecCTF</t>
+  </si>
+  <si>
+    <t>UofTCTF</t>
+  </si>
+  <si>
+    <t>les amateurs</t>
+  </si>
+  <si>
+    <t>CyberTaskForce Zero</t>
+  </si>
+  <si>
+    <t>Cwiercglowki</t>
+  </si>
+  <si>
+    <t>idk jack</t>
+  </si>
+  <si>
+    <t>flocto mad fine fr</t>
+  </si>
+  <si>
+    <t>Five Boys Cry</t>
+  </si>
+  <si>
+    <t>idek</t>
+  </si>
+  <si>
+    <t>Srdnlen</t>
+  </si>
+  <si>
+    <t>View Source</t>
+  </si>
+  <si>
+    <t>BIT CRIMINALS</t>
+  </si>
+  <si>
+    <t>neyccds</t>
+  </si>
+  <si>
+    <t>CVHS_exe</t>
+  </si>
+  <si>
+    <t>8h037</t>
+  </si>
+  <si>
+    <t>Flamingeaux</t>
+  </si>
+  <si>
+    <t>Green Onions</t>
+  </si>
+  <si>
+    <t>vEvergarden</t>
+  </si>
+  <si>
+    <t>ASU Hacking Dub B)</t>
+  </si>
+  <si>
+    <t>JuJu</t>
+  </si>
+  <si>
+    <t>cybersec_std</t>
+  </si>
+  <si>
+    <t>r0b0ter</t>
+  </si>
+  <si>
+    <t>Cheetah615</t>
+  </si>
+  <si>
+    <t>Tsuchinoko</t>
+  </si>
+  <si>
+    <t>Phantom_Troupe</t>
+  </si>
+  <si>
+    <t>no guns in meetings</t>
+  </si>
+  <si>
+    <t>nullCon</t>
+  </si>
+  <si>
+    <t>Nightingale</t>
+  </si>
+  <si>
+    <t>nek0nyaa</t>
+  </si>
+  <si>
+    <t>Titan Crew</t>
+  </si>
+  <si>
+    <t>sl1th3r</t>
+  </si>
+  <si>
+    <t>robotabc773</t>
+  </si>
+  <si>
+    <t>EverythingIsCTF</t>
+  </si>
+  <si>
+    <t>zzgrzytctf</t>
+  </si>
+  <si>
+    <t>Ethics 'R Us</t>
+  </si>
+  <si>
+    <t>GSMST CyberDragons</t>
+  </si>
+  <si>
+    <t>21S6D</t>
+  </si>
+  <si>
+    <t>Phantom Troupe</t>
+  </si>
+  <si>
+    <t>Seekers</t>
+  </si>
+  <si>
+    <t>theF0X</t>
+  </si>
+  <si>
+    <t>class_3E</t>
+  </si>
+  <si>
+    <t>fs0c13ty</t>
+  </si>
+  <si>
+    <t>CyberSpace</t>
+  </si>
+  <si>
+    <t>thehackerscrew</t>
+  </si>
+  <si>
+    <t>zemotau</t>
+  </si>
+  <si>
+    <t>0x190</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34,7 +198,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -42,7 +206,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1680047966" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -57,7 +221,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="0" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1680047966" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -65,16 +229,43 @@
         </ext>
       </extLst>
     </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1680047966" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1680047966" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -90,7 +281,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="0"/>
+          <pm:border xmlns:pm="smNativeData" id="1680047966"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1680047966"/>
         </ext>
       </extLst>
     </border>
@@ -98,8 +308,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -107,7 +318,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="0" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1680047966" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -371,18 +582,583 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="22.702703" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="n">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="n">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="n">
+        <v>7900</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="n">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="n">
+        <v>7800</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="n">
+        <v>7700</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="0" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1680047966" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -391,14 +1167,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="0" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="0" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1680047966" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1680047966" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="0" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1680047966" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>